<commit_message>
5/2/25 signup page working + allure working
</commit_message>
<xml_diff>
--- a/src/test/resources/Signup_TestData_Atutomation.xlsx
+++ b/src/test/resources/Signup_TestData_Atutomation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>TC_ID</t>
   </si>
@@ -55,7 +55,7 @@
     </r>
   </si>
   <si>
-    <t>Please fill in this field.</t>
+    <t>Please fill out this field.</t>
   </si>
   <si>
     <t>TC_03</t>
@@ -73,19 +73,13 @@
     <t>TC_05</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>a@test.com</t>
-    </r>
-  </si>
-  <si>
-    <t>A part followed by '@' should not contain the symbol':'.</t>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>a@;test.com</t>
+  </si>
+  <si>
+    <t>A part following '@' should not contain the symbol ';'.</t>
   </si>
   <si>
     <t>TC_06</t>
@@ -109,12 +103,27 @@
     <t>rahul@gmail..com</t>
   </si>
   <si>
-    <t xml:space="preserve"> is used at a wrong position in 'gmail..com'.</t>
+    <t>.' is used at a wrong position in 'gmail..com'.</t>
   </si>
   <si>
     <t>TC_09</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>rahul01_new@test.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Existing_Email</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
     <t>Aman Verma</t>
   </si>
   <si>
@@ -130,7 +139,7 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>TC_10</t>
+    <t>TC_11</t>
   </si>
   <si>
     <t>Pooja Singh</t>
@@ -145,7 +154,7 @@
     </r>
   </si>
   <si>
-    <t>TC_11</t>
+    <t>TC_12</t>
   </si>
   <si>
     <t>Rakesh Kumar</t>
@@ -160,7 +169,7 @@
     </r>
   </si>
   <si>
-    <t>TC_12</t>
+    <t>TC_13</t>
   </si>
   <si>
     <t>Neha Patel</t>
@@ -175,7 +184,7 @@
     </r>
   </si>
   <si>
-    <t>TC_13</t>
+    <t>TC_14</t>
   </si>
   <si>
     <t>Vikram Yadav</t>
@@ -190,7 +199,7 @@
     </r>
   </si>
   <si>
-    <t>TC_14</t>
+    <t>TC_15</t>
   </si>
   <si>
     <t>Suman Das</t>
@@ -205,7 +214,7 @@
     </r>
   </si>
   <si>
-    <t>TC_15</t>
+    <t>TC_16</t>
   </si>
   <si>
     <t>Arjun Mehta</t>
@@ -220,7 +229,7 @@
     </r>
   </si>
   <si>
-    <t>TC_16</t>
+    <t>TC_17</t>
   </si>
   <si>
     <t>Priya Nair</t>
@@ -235,7 +244,7 @@
     </r>
   </si>
   <si>
-    <t>TC_17</t>
+    <t>TC_18</t>
   </si>
   <si>
     <t>Mohit Agarwal</t>
@@ -250,7 +259,7 @@
     </r>
   </si>
   <si>
-    <t>TC_18</t>
+    <t>TC_19</t>
   </si>
   <si>
     <t>Kiran Reddy</t>
@@ -265,7 +274,7 @@
     </r>
   </si>
   <si>
-    <t>TC_19</t>
+    <t>TC_20</t>
   </si>
   <si>
     <t>Sameer Khan</t>
@@ -280,7 +289,7 @@
     </r>
   </si>
   <si>
-    <t>TC_20</t>
+    <t>TC_21</t>
   </si>
   <si>
     <r>
@@ -290,31 +299,13 @@
       </rPr>
       <t>rahul01_new@test.com</t>
     </r>
-  </si>
-  <si>
-    <t>TC_21</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>rahul01_new@test.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Email Address already exist!</t>
-  </si>
-  <si>
-    <t>Existing_Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -336,6 +327,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -351,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -362,6 +357,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -680,7 +681,7 @@
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -732,7 +733,7 @@
       <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -744,27 +745,27 @@
         <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
@@ -778,7 +779,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -792,7 +793,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -806,7 +807,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -820,7 +821,7 @@
         <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -834,7 +835,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -848,7 +849,7 @@
         <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -862,7 +863,7 @@
         <v>56</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -876,7 +877,7 @@
         <v>59</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
@@ -890,7 +891,7 @@
         <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -898,30 +899,27 @@
         <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" ht="16.5" customHeight="1"/>

</xml_diff>